<commit_message>
Added Material and product id
</commit_message>
<xml_diff>
--- a/data/SE-Logistik-Daten.xlsx
+++ b/data/SE-Logistik-Daten.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{F72974CE-23DA-4C1C-8FF1-E45E41AFD3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{296C9027-EDB9-4062-8329-330E34DA38C9}"/>
   <bookViews>
-    <workbookView xWindow="6735" yWindow="6915" windowWidth="18975" windowHeight="9840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5640" yWindow="3930" windowWidth="18975" windowHeight="9840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aufträge" sheetId="3" r:id="rId1"/>
@@ -608,9 +608,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A71B842-E398-47D4-951D-8819F07BF741}">
   <dimension ref="A1:AR1016"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W52" sqref="W52"/>
+      <selection pane="bottomLeft" activeCell="B42" sqref="A1:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10453,8 +10453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{429704B7-0023-4707-A09A-9A404EE4BB0C}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Data import for production facilities
</commit_message>
<xml_diff>
--- a/data/SE-Logistik-Daten.xlsx
+++ b/data/SE-Logistik-Daten.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e2851c4e9708ea5b/Documents/_Private/Uni 2022/SoftwareEngineering/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e2851c4e9708ea5b/Documents/_Private/Uni 2022/SoftwareEngineering/logistikoptimierungGitHub/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{F72974CE-23DA-4C1C-8FF1-E45E41AFD3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{296C9027-EDB9-4062-8329-330E34DA38C9}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{F72974CE-23DA-4C1C-8FF1-E45E41AFD3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5730D61A-D365-440F-BCDE-E039853DB4C8}"/>
   <bookViews>
-    <workbookView xWindow="5640" yWindow="3930" windowWidth="18975" windowHeight="9840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="6660" windowWidth="18975" windowHeight="6840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aufträge" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="78">
   <si>
     <t>Aufträge</t>
   </si>
@@ -265,6 +265,9 @@
   </si>
   <si>
     <t>#A = Nr Area, #P = Nr Produkt, Size = Größe Auftrag, Col = (YE, PU, BL, GR), Eng = (O,E,S), T = Zeit</t>
+  </si>
+  <si>
+    <t>Buffer</t>
   </si>
 </sst>
 </file>
@@ -608,9 +611,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A71B842-E398-47D4-951D-8819F07BF741}">
   <dimension ref="A1:AR1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B42" sqref="A1:B42"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10451,23 +10454,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{429704B7-0023-4707-A09A-9A404EE4BB0C}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.75" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.75" style="4" customWidth="1"/>
+    <col min="2" max="2" width="7.25" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.625" customWidth="1"/>
-    <col min="5" max="5" width="5.75" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.75" style="2" customWidth="1"/>
     <col min="9" max="9" width="5.75" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>73</v>
       </c>
@@ -10478,7 +10481,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>62</v>
       </c>
@@ -10489,7 +10492,7 @@
         <v>3.4722222222222224E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>62</v>
       </c>
@@ -10500,7 +10503,7 @@
         <v>3.4722222222222224E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>63</v>
       </c>
@@ -10511,7 +10514,7 @@
         <v>2.0833333333333333E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>64</v>
       </c>
@@ -10522,7 +10525,7 @@
         <v>2.0833333333333333E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>65</v>
       </c>
@@ -10533,7 +10536,7 @@
         <v>3.472222222222222E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>65</v>
       </c>
@@ -10544,7 +10547,7 @@
         <v>3.472222222222222E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>66</v>
       </c>
@@ -10555,7 +10558,7 @@
         <v>3.472222222222222E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>67</v>
       </c>
@@ -10566,7 +10569,7 @@
         <v>3.472222222222222E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>67</v>
       </c>
@@ -10577,7 +10580,7 @@
         <v>3.472222222222222E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>68</v>
       </c>
@@ -10588,535 +10591,583 @@
         <v>3.472222222222222E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>71</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="F13" s="5"/>
+      <c r="G13"/>
+      <c r="H13" s="5"/>
+      <c r="I13"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="4">
         <v>40</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="22">
+      <c r="E14" s="22">
         <v>3.472222222222222E-3</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>10</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G14" s="2">
-        <v>30</v>
-      </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="2">
+        <v>30</v>
+      </c>
+      <c r="I14" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="4">
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="C15" s="4">
         <v>80</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="22">
+      <c r="E15" s="22">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>40</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="G15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <v>40</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="I15" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="4">
-        <v>30</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="B16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="4">
+        <v>30</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="22">
+      <c r="E16" s="22">
         <v>2.0833333333333333E-3</v>
       </c>
-      <c r="E16">
-        <v>30</v>
-      </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16">
+        <v>30</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" s="4">
+      <c r="H16" s="2"/>
+      <c r="I16"/>
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="C17" s="4">
         <v>40</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="22">
+      <c r="E17" s="22">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>40</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="G17" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B18" s="4">
+      <c r="H17" s="2"/>
+      <c r="I17"/>
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="C18" s="4">
         <v>70</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="22">
+      <c r="E18" s="22">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>40</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="G18" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="2">
-        <v>30</v>
-      </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="2">
+        <v>30</v>
+      </c>
+      <c r="I18" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B19" s="4">
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="C19" s="4">
         <v>110</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="22">
+      <c r="E19" s="22">
         <v>1.7361111111111112E-2</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>80</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="G19" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G19" s="2">
-        <v>30</v>
-      </c>
-      <c r="H19" s="4" t="s">
+      <c r="H19" s="2">
+        <v>30</v>
+      </c>
+      <c r="I19" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B20" s="4">
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="C20" s="4">
         <v>70</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="22">
+      <c r="E20" s="22">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>40</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="G20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="2">
-        <v>30</v>
-      </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="2">
+        <v>30</v>
+      </c>
+      <c r="I20" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="4">
         <v>40</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="22">
+      <c r="E21" s="22">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>40</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="G21" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="4">
+      <c r="H21" s="2"/>
+      <c r="I21"/>
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="C22" s="4">
         <v>210</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="22">
+      <c r="E22" s="22">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>100</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="G22" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G22" s="2">
+      <c r="H22" s="2">
         <v>110</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="I22" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B23" s="4">
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="C23" s="4">
         <v>160</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="22">
+      <c r="E23" s="22">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>100</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="G23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G23" s="2">
+      <c r="H23" s="2">
         <v>60</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="I23" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B24" s="4">
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="C24" s="4">
         <v>120</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="22">
+      <c r="E24" s="22">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>80</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="G24" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G24" s="2">
+      <c r="H24" s="2">
         <v>40</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="I24" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="J24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="4">
         <v>120</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="22">
+      <c r="E25" s="22">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>80</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="G25" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G25" s="2">
+      <c r="H25" s="2">
         <v>40</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="I25" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" s="4">
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="C26" s="4">
         <v>150</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="22">
+      <c r="E26" s="22">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>80</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="G26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G26" s="2">
+      <c r="H26" s="2">
         <v>70</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="I26" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B27" s="4">
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="C27" s="4">
         <v>200</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="22">
+      <c r="E27" s="22">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>160</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="G27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G27" s="2">
+      <c r="H27" s="2">
         <v>40</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="I27" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B28" s="4">
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="C28" s="4">
         <v>200</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="22">
+      <c r="E28" s="22">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>200</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="G28" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B29" s="4">
+      <c r="H28" s="2"/>
+      <c r="I28"/>
+      <c r="J28" s="2"/>
+    </row>
+    <row r="29" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="C29" s="4">
         <v>240</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="22">
+      <c r="E29" s="22">
         <v>7.2916666666666671E-2</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>120</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="G29" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G29" s="2">
+      <c r="H29" s="2">
         <v>80</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="I29" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I29" s="2">
+      <c r="J29" s="2">
         <v>40</v>
       </c>
-      <c r="J29" s="4" t="s">
+      <c r="K29" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="4">
         <v>50</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D30" s="22">
+      <c r="E30" s="22">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>50</v>
       </c>
-      <c r="F30" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B31" s="4">
+      <c r="G30" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H30" s="2"/>
+      <c r="I30"/>
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="C31" s="4">
         <v>100</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D31" s="22">
+      <c r="E31" s="22">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>50</v>
       </c>
-      <c r="F31" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G31" s="2">
+      <c r="G31" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" s="2">
         <v>50</v>
       </c>
-      <c r="H31" s="4" t="s">
+      <c r="I31" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B32" s="4">
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="C32" s="4">
         <v>100</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="22">
+      <c r="E32" s="22">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>100</v>
       </c>
-      <c r="F32" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H32" s="2"/>
+      <c r="I32"/>
+      <c r="J32" s="2"/>
+    </row>
+    <row r="33" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="4">
         <v>60</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D33" s="22">
+      <c r="D33" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" s="22">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>60</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="G33" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B34" s="4">
+      <c r="H33" s="2"/>
+      <c r="I33"/>
+      <c r="J33" s="2"/>
+    </row>
+    <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="C34" s="4">
         <v>80</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="D34" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="22">
+      <c r="E34" s="22">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>80</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="G34" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="B35" s="4">
+      <c r="H34" s="2"/>
+      <c r="I34"/>
+      <c r="J34" s="2"/>
+    </row>
+    <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="C35" s="4">
         <v>120</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="D35" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D35" s="22">
+      <c r="E35" s="22">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>120</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="G35" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="B36" s="4">
+      <c r="H35" s="2"/>
+      <c r="I35"/>
+      <c r="J35" s="2"/>
+    </row>
+    <row r="36" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="C36" s="4">
         <v>60</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="D36" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D36" s="22">
+      <c r="E36" s="22">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>60</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="G36" s="4" t="s">
         <v>48</v>
       </c>
+      <c r="H36" s="2"/>
+      <c r="I36"/>
+      <c r="J36" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added java doc to source folder
</commit_message>
<xml_diff>
--- a/data/SE-Logistik-Daten.xlsx
+++ b/data/SE-Logistik-Daten.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e2851c4e9708ea5b/Documents/_Private/Uni 2022/SoftwareEngineering/logistikoptimierungGitHub/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{F72974CE-23DA-4C1C-8FF1-E45E41AFD3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5730D61A-D365-440F-BCDE-E039853DB4C8}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="13_ncr:1_{F72974CE-23DA-4C1C-8FF1-E45E41AFD3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B69B1423-4C56-4104-92F0-FD4B4B05F4A3}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="6660" windowWidth="18975" windowHeight="6840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21030" yWindow="3360" windowWidth="10545" windowHeight="12660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aufträge" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="82">
   <si>
     <t>Aufträge</t>
   </si>
@@ -268,6 +268,18 @@
   </si>
   <si>
     <t>Buffer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couch </t>
+  </si>
+  <si>
+    <t>BatchSize</t>
+  </si>
+  <si>
+    <t>Amount needed</t>
+  </si>
+  <si>
+    <t>Batches</t>
   </si>
 </sst>
 </file>
@@ -10454,16 +10466,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{429704B7-0023-4707-A09A-9A404EE4BB0C}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.75" style="2" customWidth="1"/>
-    <col min="2" max="2" width="7.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" style="4" customWidth="1"/>
     <col min="3" max="3" width="13.625" customWidth="1"/>
     <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.75" style="2" customWidth="1"/>
@@ -11169,6 +11181,119 @@
       <c r="I36"/>
       <c r="J36" s="2"/>
     </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B38" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="4">
+        <v>236</v>
+      </c>
+      <c r="C39">
+        <v>240</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="4">
+        <v>120</v>
+      </c>
+      <c r="C40">
+        <v>120</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" s="4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" s="4">
+        <v>80</v>
+      </c>
+      <c r="C42">
+        <v>40</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" s="4">
+        <v>40</v>
+      </c>
+      <c r="C44">
+        <v>40</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="4">
+        <v>40</v>
+      </c>
+      <c r="C45">
+        <v>40</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" s="4">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>